<commit_message>
Added review to use cases. Finalized my hours on burndown chart.
</commit_message>
<xml_diff>
--- a/project/Phase 1/Sprint1/Burndown chart.xlsx
+++ b/project/Phase 1/Sprint1/Burndown chart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joao4\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joaop\Desktop\ES\Projects\SE2122-57672-58175-57957-58210-57911\project\Phase 1\Sprint1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFC9A3C0-7279-4CA7-A708-55D18723F7D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFC5E2B7-6F14-466C-AFC4-BABBB107AB6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1515" yWindow="1515" windowWidth="14610" windowHeight="12660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -166,7 +166,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="pt-PT"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -562,22 +562,22 @@
                   <c:v>61</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>59</c:v>
+                  <c:v>55</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>55</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>47</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>32</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>15</c:v>
+                  <c:v>-9</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>7</c:v>
+                  <c:v>-21</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -979,34 +979,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="E1:R34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="S15" sqref="S15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="S20" sqref="S20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="10.5703125" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" customWidth="1"/>
+    <col min="4" max="4" width="10.5546875" customWidth="1"/>
+    <col min="5" max="5" width="9.88671875" customWidth="1"/>
     <col min="6" max="6" width="10" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" customWidth="1"/>
-    <col min="8" max="8" width="10.85546875" customWidth="1"/>
-    <col min="10" max="10" width="10.5703125" customWidth="1"/>
-    <col min="11" max="11" width="10.140625" customWidth="1"/>
-    <col min="12" max="12" width="14.5703125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="15.140625" style="1" customWidth="1"/>
-    <col min="17" max="17" width="16.42578125" customWidth="1"/>
-    <col min="18" max="18" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5546875" customWidth="1"/>
+    <col min="8" max="8" width="10.88671875" customWidth="1"/>
+    <col min="10" max="10" width="10.5546875" customWidth="1"/>
+    <col min="11" max="11" width="10.109375" customWidth="1"/>
+    <col min="12" max="12" width="14.5546875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="15.109375" style="1" customWidth="1"/>
+    <col min="17" max="17" width="16.44140625" customWidth="1"/>
+    <col min="18" max="18" width="8.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="10:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="10:17" x14ac:dyDescent="0.3">
       <c r="L1" s="8"/>
       <c r="M1" s="8"/>
     </row>
-    <row r="5" spans="10:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="10:17" x14ac:dyDescent="0.3">
       <c r="L5" s="6"/>
       <c r="M5" s="9"/>
     </row>
-    <row r="6" spans="10:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="10:17" x14ac:dyDescent="0.3">
       <c r="J6" s="2" t="s">
         <v>0</v>
       </c>
@@ -1032,7 +1032,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="10:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="10:17" x14ac:dyDescent="0.3">
       <c r="J7" s="4">
         <v>44512</v>
       </c>
@@ -1059,7 +1059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="10:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="10:17" x14ac:dyDescent="0.3">
       <c r="J8" s="4">
         <v>44513</v>
       </c>
@@ -1086,7 +1086,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="10:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="10:17" x14ac:dyDescent="0.3">
       <c r="J9" s="4">
         <v>44514</v>
       </c>
@@ -1113,7 +1113,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="10:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="10:17" x14ac:dyDescent="0.3">
       <c r="J10" s="4">
         <v>44515</v>
       </c>
@@ -1140,7 +1140,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="10:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="10:17" x14ac:dyDescent="0.3">
       <c r="J11" s="4">
         <v>44516</v>
       </c>
@@ -1167,7 +1167,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="10:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="10:17" x14ac:dyDescent="0.3">
       <c r="J12" s="4">
         <v>44517</v>
       </c>
@@ -1194,7 +1194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="10:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="10:17" x14ac:dyDescent="0.3">
       <c r="J13" s="4">
         <v>44518</v>
       </c>
@@ -1221,7 +1221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="10:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="10:17" x14ac:dyDescent="0.3">
       <c r="J14" s="4">
         <v>44519</v>
       </c>
@@ -1248,7 +1248,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="10:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="10:17" x14ac:dyDescent="0.3">
       <c r="J15" s="4">
         <v>44520</v>
       </c>
@@ -1262,7 +1262,9 @@
       <c r="M15" s="2">
         <v>0</v>
       </c>
-      <c r="N15" s="2"/>
+      <c r="N15" s="2">
+        <v>0</v>
+      </c>
       <c r="O15" s="2">
         <v>0</v>
       </c>
@@ -1273,7 +1275,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="10:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="10:17" x14ac:dyDescent="0.3">
       <c r="J16" s="4">
         <v>44521</v>
       </c>
@@ -1287,7 +1289,9 @@
       <c r="M16" s="2">
         <v>0</v>
       </c>
-      <c r="N16" s="2"/>
+      <c r="N16" s="3">
+        <v>0</v>
+      </c>
       <c r="O16" s="2">
         <v>0</v>
       </c>
@@ -1298,7 +1302,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="5:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="5:18" x14ac:dyDescent="0.3">
       <c r="J17" s="4">
         <v>44522</v>
       </c>
@@ -1312,7 +1316,9 @@
       <c r="M17" s="2">
         <v>0</v>
       </c>
-      <c r="N17" s="2"/>
+      <c r="N17" s="3">
+        <v>0</v>
+      </c>
       <c r="O17" s="2">
         <v>0</v>
       </c>
@@ -1323,7 +1329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="5:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="5:18" x14ac:dyDescent="0.3">
       <c r="J18" s="4">
         <v>44523</v>
       </c>
@@ -1337,7 +1343,9 @@
       <c r="M18" s="2">
         <v>3</v>
       </c>
-      <c r="N18" s="2"/>
+      <c r="N18" s="3">
+        <v>0</v>
+      </c>
       <c r="O18" s="2">
         <v>0</v>
       </c>
@@ -1348,7 +1356,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="5:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="5:18" x14ac:dyDescent="0.3">
       <c r="J19" s="4">
         <v>44524</v>
       </c>
@@ -1362,7 +1370,9 @@
       <c r="M19" s="2">
         <v>1</v>
       </c>
-      <c r="N19" s="2"/>
+      <c r="N19" s="3">
+        <v>0</v>
+      </c>
       <c r="O19" s="2">
         <v>0</v>
       </c>
@@ -1373,7 +1383,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="5:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="5:18" x14ac:dyDescent="0.3">
       <c r="J20" s="4">
         <v>44525</v>
       </c>
@@ -1387,7 +1397,9 @@
       <c r="M20" s="2">
         <v>0</v>
       </c>
-      <c r="N20" s="2"/>
+      <c r="N20" s="3">
+        <v>0</v>
+      </c>
       <c r="O20" s="2">
         <v>0</v>
       </c>
@@ -1398,7 +1410,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="5:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="5:18" x14ac:dyDescent="0.3">
       <c r="J21" s="4">
         <v>44526</v>
       </c>
@@ -1412,7 +1424,9 @@
       <c r="M21" s="2">
         <v>2</v>
       </c>
-      <c r="N21" s="2"/>
+      <c r="N21" s="3">
+        <v>0</v>
+      </c>
       <c r="O21" s="2">
         <v>0</v>
       </c>
@@ -1423,7 +1437,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="5:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="5:18" x14ac:dyDescent="0.3">
       <c r="J22" s="4">
         <v>44527</v>
       </c>
@@ -1437,7 +1451,9 @@
       <c r="M22" s="2">
         <v>0</v>
       </c>
-      <c r="N22" s="2"/>
+      <c r="N22" s="3">
+        <v>0</v>
+      </c>
       <c r="O22" s="2">
         <v>0</v>
       </c>
@@ -1448,7 +1464,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="5:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="5:18" x14ac:dyDescent="0.3">
       <c r="J23" s="4">
         <v>44528</v>
       </c>
@@ -1462,7 +1478,9 @@
       <c r="M23" s="2">
         <v>0</v>
       </c>
-      <c r="N23" s="2"/>
+      <c r="N23" s="3">
+        <v>0</v>
+      </c>
       <c r="O23" s="2">
         <v>0</v>
       </c>
@@ -1473,7 +1491,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="5:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="5:18" x14ac:dyDescent="0.3">
       <c r="J24" s="4">
         <v>44529</v>
       </c>
@@ -1487,7 +1505,9 @@
       <c r="M24" s="2">
         <v>0</v>
       </c>
-      <c r="N24" s="2"/>
+      <c r="N24" s="3">
+        <v>0</v>
+      </c>
       <c r="O24" s="2">
         <v>0</v>
       </c>
@@ -1498,7 +1518,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="5:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="5:18" x14ac:dyDescent="0.3">
       <c r="J25" s="4">
         <v>44530</v>
       </c>
@@ -1512,7 +1532,9 @@
       <c r="M25" s="2">
         <v>0</v>
       </c>
-      <c r="N25" s="2"/>
+      <c r="N25" s="3">
+        <v>0</v>
+      </c>
       <c r="O25" s="2">
         <v>0</v>
       </c>
@@ -1523,7 +1545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="5:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="5:18" x14ac:dyDescent="0.3">
       <c r="J26" s="4">
         <v>44531</v>
       </c>
@@ -1532,12 +1554,14 @@
       </c>
       <c r="L26" s="7">
         <f t="shared" si="0"/>
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="M26" s="2">
         <v>0</v>
       </c>
-      <c r="N26" s="2"/>
+      <c r="N26" s="2">
+        <v>4</v>
+      </c>
       <c r="O26" s="2">
         <v>2</v>
       </c>
@@ -1548,7 +1572,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="5:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="5:18" x14ac:dyDescent="0.3">
       <c r="J27" s="4">
         <v>44532</v>
       </c>
@@ -1557,12 +1581,14 @@
       </c>
       <c r="L27" s="7">
         <f t="shared" si="0"/>
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="M27" s="2">
         <v>2</v>
       </c>
-      <c r="N27" s="2"/>
+      <c r="N27" s="2">
+        <v>3</v>
+      </c>
       <c r="O27" s="2">
         <v>2</v>
       </c>
@@ -1573,7 +1599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="5:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="5:18" x14ac:dyDescent="0.3">
       <c r="J28" s="4">
         <v>44533</v>
       </c>
@@ -1582,12 +1608,14 @@
       </c>
       <c r="L28" s="7">
         <f t="shared" si="0"/>
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="M28" s="2">
         <v>2</v>
       </c>
-      <c r="N28" s="2"/>
+      <c r="N28" s="2">
+        <v>5</v>
+      </c>
       <c r="O28" s="2">
         <v>3</v>
       </c>
@@ -1598,7 +1626,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="5:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="5:18" x14ac:dyDescent="0.3">
       <c r="J29" s="4">
         <v>44534</v>
       </c>
@@ -1607,12 +1635,14 @@
       </c>
       <c r="L29" s="7">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="M29" s="2">
         <v>3</v>
       </c>
-      <c r="N29" s="2"/>
+      <c r="N29" s="2">
+        <v>5</v>
+      </c>
       <c r="O29" s="2">
         <v>4</v>
       </c>
@@ -1623,7 +1653,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="5:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="5:18" x14ac:dyDescent="0.3">
       <c r="J30" s="4">
         <v>44535</v>
       </c>
@@ -1632,12 +1662,14 @@
       </c>
       <c r="L30" s="7">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>-9</v>
       </c>
       <c r="M30" s="2">
         <v>3</v>
       </c>
-      <c r="N30" s="2"/>
+      <c r="N30" s="2">
+        <v>7</v>
+      </c>
       <c r="O30" s="2">
         <v>4</v>
       </c>
@@ -1648,7 +1680,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="5:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="5:18" x14ac:dyDescent="0.3">
       <c r="J31" s="4">
         <v>44536</v>
       </c>
@@ -1657,12 +1689,14 @@
       </c>
       <c r="L31" s="7">
         <f t="shared" ref="L31" si="1">L30-SUM(M31:Q31)</f>
-        <v>7</v>
+        <v>-21</v>
       </c>
       <c r="M31" s="3">
         <v>1</v>
       </c>
-      <c r="N31" s="3"/>
+      <c r="N31" s="3">
+        <v>4</v>
+      </c>
       <c r="O31" s="3">
         <v>2</v>
       </c>
@@ -1673,7 +1707,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="5:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="5:18" x14ac:dyDescent="0.3">
       <c r="E32" s="5"/>
       <c r="M32" s="1">
         <f>SUM(M7:M31)</f>
@@ -1681,7 +1715,7 @@
       </c>
       <c r="N32" s="1">
         <f t="shared" ref="N32:Q32" si="2">SUM(N7:N31)</f>
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="O32" s="1">
         <f t="shared" si="2"/>
@@ -1699,13 +1733,13 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="5:18" x14ac:dyDescent="0.25">
+    <row r="33" spans="5:18" x14ac:dyDescent="0.3">
       <c r="E33" s="5"/>
       <c r="R33" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="5:18" x14ac:dyDescent="0.25">
+    <row r="34" spans="5:18" x14ac:dyDescent="0.3">
       <c r="E34" s="5"/>
       <c r="N34" s="11"/>
       <c r="R34" s="10">

</xml_diff>